<commit_message>
updated final score data
</commit_message>
<xml_diff>
--- a/NL/CHN.xlsx
+++ b/NL/CHN.xlsx
@@ -93553,10 +93553,10 @@
         <v>953</v>
       </c>
       <c r="D10" t="s">
-        <v>951</v>
+        <v>1317</v>
       </c>
       <c r="E10" t="s">
-        <v>1086</v>
+        <v>1621</v>
       </c>
     </row>
   </sheetData>
@@ -93704,10 +93704,10 @@
         <v>2022.0</v>
       </c>
       <c r="C10" t="s">
-        <v>1361</v>
+        <v>1251</v>
       </c>
       <c r="D10" t="s">
-        <v>1273</v>
+        <v>1257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>